<commit_message>
added new data set
</commit_message>
<xml_diff>
--- a/assignment_data_4.xlsx
+++ b/assignment_data_4.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\next-best-position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E80E1B5B-966A-48E8-8B4B-2EB0C8A7AE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ED838D-4DCE-4DC5-888C-C71CD8B62903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1B66F183-0BCD-4F97-8FF8-4BD92C1308AE}"/>
   </bookViews>
   <sheets>
-    <sheet name="employees" sheetId="1" r:id="rId1"/>
-    <sheet name="open positions" sheetId="2" r:id="rId2"/>
-    <sheet name="formulas" sheetId="3" r:id="rId3"/>
+    <sheet name="matches" sheetId="4" r:id="rId1"/>
+    <sheet name="employees" sheetId="1" r:id="rId2"/>
+    <sheet name="open positions" sheetId="2" r:id="rId3"/>
+    <sheet name="formulas" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">employees!$A$1:$D$101</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'open positions'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">employees!$A$1:$D$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'open positions'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="11">
   <si>
     <t>employee_id</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>region</t>
+  </si>
+  <si>
+    <t>position_id</t>
   </si>
 </sst>
 </file>
@@ -412,10 +416,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B8DB73-2F44-4CE4-8C25-DBC453EF110E}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1067</v>
+      </c>
+      <c r="B2">
+        <v>1016</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1134</v>
+      </c>
+      <c r="B3">
+        <v>1016</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1201</v>
+      </c>
+      <c r="B4">
+        <v>1016</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1268</v>
+      </c>
+      <c r="B5">
+        <v>1016</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1067</v>
+      </c>
+      <c r="B6">
+        <v>1037</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1134</v>
+      </c>
+      <c r="B7">
+        <v>1037</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1201</v>
+      </c>
+      <c r="B8">
+        <v>1037</v>
+      </c>
+      <c r="C8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1268</v>
+      </c>
+      <c r="B9">
+        <v>1037</v>
+      </c>
+      <c r="C9">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1067</v>
+      </c>
+      <c r="B10">
+        <v>1033</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1134</v>
+      </c>
+      <c r="B11">
+        <v>1033</v>
+      </c>
+      <c r="C11">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1201</v>
+      </c>
+      <c r="B12">
+        <v>1033</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1268</v>
+      </c>
+      <c r="B13">
+        <v>1033</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1067</v>
+      </c>
+      <c r="B14">
+        <v>1013</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1134</v>
+      </c>
+      <c r="B15">
+        <v>1013</v>
+      </c>
+      <c r="C15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1201</v>
+      </c>
+      <c r="B16">
+        <v>1013</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1268</v>
+      </c>
+      <c r="B17">
+        <v>1013</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2614F31-0953-43BE-ABDC-2F399F76A8BE}">
   <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -2199,7 +2406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359C2FAD-099F-46C8-A0D9-E07FF297F409}">
   <dimension ref="A1:D101"/>
   <sheetViews>
@@ -3632,7 +3839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B4741E-6330-4828-AC4B-75AE610DD2DF}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -3670,7 +3877,7 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">TODAY()+RANDBETWEEN(1,180)</f>
-        <v>45475</v>
+        <v>45433</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3680,7 +3887,7 @@
       </c>
       <c r="F2" s="1">
         <f ca="1">TODAY()+RANDBETWEEN(14,365)</f>
-        <v>45595</v>
+        <v>45562</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3690,7 +3897,7 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3" ca="1" si="0">TODAY()+RANDBETWEEN(14,365)</f>
-        <v>45440</v>
+        <v>45619</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -3701,7 +3908,7 @@
       </c>
       <c r="F3" s="1">
         <f ca="1">TODAY()+RANDBETWEEN(14,365)</f>
-        <v>45470</v>
+        <v>45518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>